<commit_message>
refactor to version 1.1.6
</commit_message>
<xml_diff>
--- a/data/vlsp2016/eda/dev/column-1-analyze.xlsx
+++ b/data/vlsp2016/eda/dev/column-1-analyze.xlsx
@@ -41,25 +41,25 @@
     <t>CH</t>
   </si>
   <si>
-    <t>,, ., ", ..., :, -, (, ), ?, !</t>
+    <t>,, ., ", ..., :, -, ), (, ?, !</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>của, trong, với, cho, ở, để, về, đến, từ, trên</t>
+    <t>của, trong, với, cho, ở, để, về, từ, đến, trên</t>
   </si>
   <si>
     <t>FW</t>
   </si>
   <si>
-    <t>oxy, marketing, shop, cas, nilông, Oxy, Moran, radio, êkip, Games</t>
+    <t>oxy, marketing, shop, nilông, cas, Moran, Oxy, radio, Games, vali</t>
   </si>
   <si>
     <t>I</t>
   </si>
   <si>
-    <t>ơi, Ôi, ư, ạ, nha, Ồ, Ừ, Vâng, nhỉ, thay</t>
+    <t>ơi, Ôi, ư, ạ, Ồ, Ừ, Vâng, nha, nhỉ, Hỡi</t>
   </si>
   <si>
     <t>L</t>
@@ -83,31 +83,31 @@
     <t>Nc</t>
   </si>
   <si>
-    <t>người, chị, anh, bà, ông, cái, con, chiếc, cô, Anh</t>
+    <t>người, chị, anh, bà, ông, cái, con, cô, chiếc, Anh</t>
   </si>
   <si>
     <t>Np</t>
   </si>
   <si>
-    <t>Thuỳ, VN, Mỹ, Nguyễn, Trâm, Khiêm, Thành, HCM, miền, Văn</t>
+    <t>Thuỳ, VN, Mỹ, Nguyễn, Trâm, Khiêm, Thành, miền, Văn, HCM</t>
   </si>
   <si>
     <t>Nu</t>
   </si>
   <si>
-    <t>đồng, phút, lít, g, giờ, ha, USD, m, tấn, ký</t>
+    <t>đồng, phút, lít, g, giờ, ha, m, USD, tấn, giây</t>
   </si>
   <si>
     <t>Ny</t>
   </si>
   <si>
-    <t>TP., NTLS, ĐDV, BS, ĐĐV, CCV, TP, UBND, Q., AIDS</t>
+    <t>TP., NTLS, ĐDV, BS, ĐĐV, CCV, TP, Q., AIDS, UBND</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
-    <t>mình, tôi, đó, này, ấy, họ, Tôi, chúng tôi, đây, gì</t>
+    <t>mình, tôi, đó, này, ấy, họ, Tôi, đây, chúng tôi, gì</t>
   </si>
   <si>
     <t>R</t>
@@ -119,7 +119,7 @@
     <t>T</t>
   </si>
   <si>
-    <t>cả, chính, rồi, thôi, ngay, thật, đâu, mà, sao, nào</t>
+    <t>cả, chính, rồi, thôi, ngay, thật, đâu, mà, nào, sao</t>
   </si>
   <si>
     <t>V</t>
@@ -131,13 +131,13 @@
     <t>X</t>
   </si>
   <si>
-    <t>một mình, vì sao, làm sao, Tại sao, như vậy, Vì sao, ngày càng, vừa qua, vậy mà, có lẽ</t>
+    <t>vì sao, một mình, như vậy, làm sao, Tại sao, Vì sao, ngày càng, vừa qua, thế nào, có lẽ</t>
   </si>
   <si>
     <t>Z</t>
   </si>
   <si>
-    <t>đa, phó, Phó, phi, viên</t>
+    <t>đa, phó, phi, Phó, viên</t>
   </si>
 </sst>
 </file>

</xml_diff>